<commit_message>
Adding few test cases along with nwe custom utlities
</commit_message>
<xml_diff>
--- a/config/TestData.xlsx
+++ b/config/TestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajas\git\repository\CustomHybridFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e910955fcfc76e87/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C09D9-21B9-4995-A7F4-8DAC6BEE68D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{7D837D26-D4DD-4E2E-80D6-0DE5D4532E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A5BD04E-4EDC-4105-A88F-124116F8384D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1C44674A-58AF-4570-9B24-52073566F4FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1C44674A-58AF-4570-9B24-52073566F4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
+    <sheet name="pimAddEmpoyeeData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Admin</t>
   </si>
@@ -43,6 +44,30 @@
   </si>
   <si>
     <t>sri2341</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Charan</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Kumar</t>
   </si>
 </sst>
 </file>
@@ -98,9 +123,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +163,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +269,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34539E4C-97E1-41DD-BC40-55C45F9C12E7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,4 +457,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B862CA0A-E45B-4048-915A-0F07B9594E0C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>